<commit_message>
Cleaning code for submission
</commit_message>
<xml_diff>
--- a/data/P_Type.xlsx
+++ b/data/P_Type.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\home.ansatt.ntnu.no\romainb\Documents\6. Papers\6. Dynamic MFA Al in Passenger cars\Dynamic-MFA-Al-in-Passenger-Cars\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82134FDD-E314-420A-9095-E844B6B80916}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8258825A-844C-4181-985B-236E78287FF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{A1E14EBA-2D53-4191-B00D-F0359C507412}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Cover" sheetId="2" r:id="rId1"/>
     <sheet name="Data" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -357,6 +357,2301 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>P_Type parameter</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$A$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ICEV</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Data!$CX$1:$EV$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="51"/>
+                <c:pt idx="0">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2021</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2022</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2023</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2024</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2025</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2026</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2027</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2028</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2029</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2030</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2031</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2032</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2033</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2034</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2035</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2036</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2037</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2038</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2039</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>2040</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>2041</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>2042</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>2043</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>2044</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>2045</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>2046</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>2047</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>2049</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>2050</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$CX$2:$EV$2</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="51"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.99</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-51A3-4E48-A46D-6D2586296066}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>HEV</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Data!$CX$1:$EV$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="51"/>
+                <c:pt idx="0">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2021</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2022</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2023</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2024</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2025</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2026</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2027</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2028</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2029</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2030</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2031</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2032</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2033</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2034</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2035</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2036</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2037</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2038</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2039</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>2040</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>2041</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>2042</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>2043</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>2044</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>2045</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>2046</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>2047</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>2049</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>2050</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$CX$3:$EV$3</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="51"/>
+                <c:pt idx="0">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>1.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-51A3-4E48-A46D-6D2586296066}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>PHEV</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Data!$CX$1:$EV$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="51"/>
+                <c:pt idx="0">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2021</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2022</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2023</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2024</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2025</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2026</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2027</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2028</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2029</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2030</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2031</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2032</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2033</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2034</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2035</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2036</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2037</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2038</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2039</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>2040</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>2041</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>2042</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>2043</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>2044</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>2045</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>2046</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>2047</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>2049</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>2050</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$CX$4:$EV$4</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="51"/>
+                <c:pt idx="0">
+                  <c:v>1.8786440252787182</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.8786440252787182</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.8786440252787182</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.8786440252787182</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.8786440252787182</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.8786440252787182</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.8786440252787182</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.8786440252787182</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.8786440252787182</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.8786440252787182</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.8786440252787182</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.8786440252787182</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.8786440252787182</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.8786440252787182</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.8786440252787182</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.8786440252787182</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.8786440252787182</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.8786440252787182</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.8786440252787182</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.8786440252787182</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.8786440252787182</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.8626892244360942</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.8467344235934702</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.8307796227508462</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.8148248219082221</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.7988700210655981</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1.7829152202229741</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.7669604193803501</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.7510056185377261</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.7350508176951021</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.719096016852478</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1.703141216009854</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1.68718641516723</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1.671231614324606</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1.655276813481982</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1.639322012639358</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1.6233672117967339</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1.6074124109541099</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1.5914576101114859</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1.5755028092688619</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1.5595480084262379</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1.5435932075836138</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1.5276384067409898</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1.5116836058983658</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1.4957288050557418</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1.4797740042131178</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1.4638192033704938</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1.4478644025278697</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1.4319096016852457</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1.4159548008426217</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>1.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-51A3-4E48-A46D-6D2586296066}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>BEV</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Data!$CX$1:$EV$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="51"/>
+                <c:pt idx="0">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2019</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2021</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2022</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2023</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2024</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2025</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2026</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2027</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2028</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2029</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2030</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2031</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2032</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2033</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2034</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2035</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2036</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2037</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2038</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2039</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>2040</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>2041</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>2042</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>2043</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>2044</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>2045</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>2046</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>2047</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>2049</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>2050</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$CX$5:$EV$5</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="51"/>
+                <c:pt idx="0">
+                  <c:v>1.9700357533836292</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.9700357533836292</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.9700357533836292</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.9700357533836292</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.9700357533836292</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.9700357533836292</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.9700357533836292</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.9700357533836292</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.9700357533836292</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.9700357533836292</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.9700357533836292</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.9700357533836292</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.9700357533836292</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.9700357533836292</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.9700357533836292</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.9700357533836292</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.9700357533836292</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.9700357533836292</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.9700357533836292</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.9700357533836292</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.9700357533836292</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.9577012282708417</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.9453667031580542</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.9330321780452666</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.9206976529324791</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.9083631278196915</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1.896028602706904</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.8836940775941164</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.8713595524813289</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.8590250273685414</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.8466905022557538</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1.8343559771429663</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1.8220214520301787</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1.8096869269173912</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1.7973524018046036</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1.7850178766918161</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1.7726833515790286</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1.760348826466241</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1.7480143013534535</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1.7356797762406659</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1.7233452511278784</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1.7110107260150909</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1.6986762009023033</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1.6863416757895158</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1.6740071506767282</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1.6616726255639407</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1.6493381004511531</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1.6370035753383656</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1.6246690502255781</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1.6123345251127905</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>1.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-51A3-4E48-A46D-6D2586296066}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1265184936"/>
+        <c:axId val="1265185592"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1265184936"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1265185592"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1265185592"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1265184936"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>131</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>138</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D587B3C3-D475-79FD-C083-679561EDDB17}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1159,11 +3454,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBF9B55B-12FE-418D-9CE2-848557F20CC6}">
   <dimension ref="A1:EX5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="DL2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="DM2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="EV6" sqref="EV6"/>
+      <selection pane="bottomRight" activeCell="DW16" sqref="DW16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2489,7 +4784,7 @@
         <v>0</v>
       </c>
       <c r="CX3" s="3">
-        <v>0</v>
+        <v>1.2</v>
       </c>
       <c r="CY3" s="3">
         <v>1.2</v>
@@ -2997,7 +5292,7 @@
         <v>0</v>
       </c>
       <c r="CX4" s="3">
-        <v>0</v>
+        <v>1.8786440252787182</v>
       </c>
       <c r="CY4" s="3">
         <v>1.8786440252787182</v>
@@ -3064,7 +5359,7 @@
         <v>1.8626892244360942</v>
       </c>
       <c r="DT4" s="3">
-        <f t="shared" ref="DS2:EU4" si="7">DS4+($EV4-$DR4)/30</f>
+        <f t="shared" ref="DT4:EU4" si="7">DS4+($EV4-$DR4)/30</f>
         <v>1.8467344235934702</v>
       </c>
       <c r="DU4" s="3">
@@ -3534,7 +5829,7 @@
         <v>0</v>
       </c>
       <c r="CX5" s="3">
-        <v>0</v>
+        <v>1.9700357533836292</v>
       </c>
       <c r="CY5" s="3">
         <v>1.9700357533836292</v>
@@ -3719,5 +6014,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>